<commit_message>
No se me guardo bien
</commit_message>
<xml_diff>
--- a/P1/Usability-review-template.xlsx
+++ b/P1/Usability-review-template.xlsx
@@ -723,7 +723,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
   <si>
     <t xml:space="preserve">Usability review (Español)</t>
   </si>
@@ -933,6 +933,9 @@
   </si>
   <si>
     <t xml:space="preserve">Se solicita una cantidad mínima de información y, cuando se proporciona la justificación necesaria para solicitar información (por ejemplo, fecha de nacimiento, número de teléfono)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si se solicita información es para hacer la reserva o para  crearse una cuenta</t>
   </si>
   <si>
     <t xml:space="preserve">Los campos de formulario requeridos y opcionales están claramente indicados</t>
@@ -5090,7 +5093,9 @@
         <v>#REF!</v>
       </c>
       <c r="H69" s="7"/>
-      <c r="I69" s="41"/>
+      <c r="I69" s="41" t="s">
+        <v>69</v>
+      </c>
       <c r="J69" s="7"/>
       <c r="K69" s="14">
         <v>2</v>
@@ -5135,7 +5140,7 @@
         <v>27</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71" s="40" t="s">
@@ -5152,7 +5157,7 @@
       </c>
       <c r="H71" s="7"/>
       <c r="I71" s="41" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J71" s="7"/>
       <c r="K71" s="14">
@@ -5198,7 +5203,7 @@
         <v>28</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="40" t="s">
@@ -5259,7 +5264,7 @@
         <v>29</v>
       </c>
       <c r="B75" s="39" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="40" t="s">
@@ -5276,7 +5281,7 @@
       </c>
       <c r="H75" s="7"/>
       <c r="I75" s="41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J75" s="7"/>
       <c r="K75" s="14">
@@ -5317,7 +5322,7 @@
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C77" s="36"/>
       <c r="D77" s="53"/>
@@ -5355,7 +5360,7 @@
         <v>30</v>
       </c>
       <c r="B79" s="39" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="40" t="s">
@@ -5372,7 +5377,7 @@
       </c>
       <c r="H79" s="7"/>
       <c r="I79" s="41" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J79" s="7"/>
       <c r="K79" s="14">
@@ -5418,7 +5423,7 @@
         <v>31</v>
       </c>
       <c r="B81" s="39" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C81" s="7"/>
       <c r="D81" s="40" t="s">
@@ -5479,7 +5484,7 @@
         <v>32</v>
       </c>
       <c r="B83" s="39" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="40" t="s">
@@ -5496,7 +5501,7 @@
       </c>
       <c r="H83" s="7"/>
       <c r="I83" s="41" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J83" s="7"/>
       <c r="K83" s="14">
@@ -5542,7 +5547,7 @@
         <v>33</v>
       </c>
       <c r="B85" s="39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="40" t="s">
@@ -5598,7 +5603,7 @@
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C87" s="36"/>
       <c r="D87" s="53"/>
@@ -5636,7 +5641,7 @@
         <v>34</v>
       </c>
       <c r="B89" s="39" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="40" t="s">
@@ -5653,7 +5658,7 @@
       </c>
       <c r="H89" s="7"/>
       <c r="I89" s="41" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J89" s="7"/>
       <c r="K89" s="14">
@@ -5699,7 +5704,7 @@
         <v>35</v>
       </c>
       <c r="B91" s="39" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="40" t="s">
@@ -5760,7 +5765,7 @@
         <v>36</v>
       </c>
       <c r="B93" s="39" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93" s="40" t="s">
@@ -5777,7 +5782,7 @@
       </c>
       <c r="H93" s="7"/>
       <c r="I93" s="41" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J93" s="7"/>
       <c r="K93" s="14">
@@ -5823,7 +5828,7 @@
         <v>37</v>
       </c>
       <c r="B95" s="39" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C95" s="7"/>
       <c r="D95" s="40" t="s">
@@ -5840,7 +5845,7 @@
       </c>
       <c r="H95" s="7"/>
       <c r="I95" s="41" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J95" s="7"/>
       <c r="K95" s="14">
@@ -5886,7 +5891,7 @@
         <v>38</v>
       </c>
       <c r="B97" s="39" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C97" s="7"/>
       <c r="D97" s="40" t="s">
@@ -5903,7 +5908,7 @@
       </c>
       <c r="H97" s="7"/>
       <c r="I97" s="41" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J97" s="7"/>
       <c r="K97" s="14">
@@ -5944,7 +5949,7 @@
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C99" s="36"/>
       <c r="D99" s="53"/>
@@ -5982,7 +5987,7 @@
         <v>39</v>
       </c>
       <c r="B101" s="39" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C101" s="7"/>
       <c r="D101" s="40" t="s">
@@ -6043,7 +6048,7 @@
         <v>40</v>
       </c>
       <c r="B103" s="39" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C103" s="7"/>
       <c r="D103" s="40" t="s">
@@ -6060,7 +6065,7 @@
       </c>
       <c r="H103" s="7"/>
       <c r="I103" s="41" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J103" s="7"/>
       <c r="K103" s="14">
@@ -6106,7 +6111,7 @@
         <v>41</v>
       </c>
       <c r="B105" s="39" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C105" s="7"/>
       <c r="D105" s="40" t="s">
@@ -6123,7 +6128,7 @@
       </c>
       <c r="H105" s="7"/>
       <c r="I105" s="41" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J105" s="7"/>
       <c r="K105" s="14">
@@ -6169,7 +6174,7 @@
         <v>42</v>
       </c>
       <c r="B107" s="39" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C107" s="7"/>
       <c r="D107" s="40" t="s">
@@ -6186,7 +6191,7 @@
       </c>
       <c r="H107" s="7"/>
       <c r="I107" s="41" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J107" s="7"/>
       <c r="K107" s="14">
@@ -6227,7 +6232,7 @@
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="34" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C109" s="36"/>
       <c r="D109" s="53"/>
@@ -6265,7 +6270,7 @@
         <v>43</v>
       </c>
       <c r="B111" s="39" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C111" s="21"/>
       <c r="D111" s="40" t="s">
@@ -6348,7 +6353,7 @@
         <v>44</v>
       </c>
       <c r="B113" s="39" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C113" s="21"/>
       <c r="D113" s="58" t="s">
@@ -6365,7 +6370,7 @@
       </c>
       <c r="H113" s="21"/>
       <c r="I113" s="41" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J113" s="21"/>
       <c r="K113" s="31">
@@ -6433,7 +6438,7 @@
         <v>45</v>
       </c>
       <c r="B115" s="39" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C115" s="21"/>
       <c r="D115" s="40" t="s">
@@ -6450,7 +6455,7 @@
       </c>
       <c r="H115" s="21"/>
       <c r="I115" s="41" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J115" s="21"/>
       <c r="K115" s="31">
@@ -6502,7 +6507,7 @@
     </row>
     <row r="117" ht="24" customHeight="1">
       <c r="A117" s="62" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B117" s="63"/>
       <c r="C117" s="64"/>
@@ -6635,10 +6640,10 @@
     </row>
     <row r="125" ht="13.5" customHeight="1">
       <c r="B125" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C125" s="78" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D125" s="79"/>
       <c r="E125" s="7"/>
@@ -6655,7 +6660,7 @@
       <c r="A126" s="7"/>
       <c r="B126" s="80"/>
       <c r="C126" s="81" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D126" s="82"/>
       <c r="E126" s="82"/>
@@ -17185,7 +17190,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00DB00AC-000C-44D7-95EE-003600A800D4}">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00A600C7-006B-46CE-9936-00B2003E0095}">
             <xm:f>"Enter score"</xm:f>
             <x14:dxf>
               <font/>
@@ -17226,19 +17231,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00FD0094-0071-4449-AF90-00E400320031}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt=" - " showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005E0098-000E-4262-BF88-00A2009E00D3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt=" - " showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$Q$1:$Q$8</xm:f>
           </x14:formula1>
           <xm:sqref>D18 D54 D74 D96</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CF007E-0043-42B6-9B03-006C006400F6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="Invalid score entered - Score must be one of:&#10;&#10;Very poor&#10;Poor&#10;Moderate&#10;Good&#10;Excellent&#10;N/A" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EC00F8-0049-4DE2-8361-00B700CE00E6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="Invalid score entered - Score must be one of:&#10;&#10;Very poor&#10;Poor&#10;Moderate&#10;Good&#10;Excellent&#10;N/A" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$Q$1:$Q$8</xm:f>
           </x14:formula1>
           <xm:sqref>D24 D32</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D50000-006B-4101-9234-00CD00D700F1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="Invalid score entered - Score must be one of:&#10;&#10;Very poor&#10;Poor&#10;Moderate&#10;Good&#10;Excellent&#10;N/A" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00200035-00B9-468B-B339-006400BD00C1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="Invalid score entered - Score must be one of:&#10;&#10;Very poor&#10;Poor&#10;Moderate&#10;Good&#10;Excellent&#10;N/A" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$Q$1:$Q$7</xm:f>
           </x14:formula1>
@@ -17281,7 +17286,7 @@
   <sheetData>
     <row r="1" ht="23.25" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -17338,7 +17343,7 @@
     </row>
     <row r="3" ht="24" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
@@ -17516,7 +17521,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="40" t="s">
@@ -17591,7 +17596,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="40" t="s">
@@ -17664,7 +17669,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="40" t="s">
@@ -17733,7 +17738,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="40" t="s">
@@ -17799,7 +17804,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="40" t="s">
@@ -17897,7 +17902,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="40" t="s">
@@ -17961,7 +17966,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="40" t="s">
@@ -18026,7 +18031,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="40" t="s">
@@ -18125,7 +18130,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="43" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="40" t="s">
@@ -18193,7 +18198,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="43" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="40" t="s">
@@ -18254,7 +18259,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="43" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="40" t="s">
@@ -18309,7 +18314,7 @@
         <v>12</v>
       </c>
       <c r="B35" s="43" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="40" t="s">
@@ -18370,7 +18375,7 @@
         <v>13</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="40" t="s">
@@ -18431,7 +18436,7 @@
         <v>14</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="40" t="s">
@@ -18499,7 +18504,7 @@
         <v>15</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="40" t="s">
@@ -18560,7 +18565,7 @@
         <v>16</v>
       </c>
       <c r="B43" s="43" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="40" t="s">
@@ -18621,7 +18626,7 @@
         <v>17</v>
       </c>
       <c r="B45" s="43" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="40" t="s">
@@ -18715,7 +18720,7 @@
         <v>18</v>
       </c>
       <c r="B49" s="43" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="40" t="s">
@@ -18776,7 +18781,7 @@
         <v>19</v>
       </c>
       <c r="B51" s="43" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="40" t="s">
@@ -18837,7 +18842,7 @@
         <v>20</v>
       </c>
       <c r="B53" s="43" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="40" t="s">
@@ -18898,7 +18903,7 @@
         <v>21</v>
       </c>
       <c r="B55" s="43" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="40" t="s">
@@ -18992,7 +18997,7 @@
         <v>22</v>
       </c>
       <c r="B59" s="43" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="40" t="s">
@@ -19053,7 +19058,7 @@
         <v>23</v>
       </c>
       <c r="B61" s="43" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C61" s="7"/>
       <c r="D61" s="40" t="s">
@@ -19114,7 +19119,7 @@
         <v>24</v>
       </c>
       <c r="B63" s="43" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="40" t="s">
@@ -19208,7 +19213,7 @@
         <v>25</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="40" t="s">
@@ -19269,7 +19274,7 @@
         <v>26</v>
       </c>
       <c r="B69" s="43" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="40" t="s">
@@ -19330,7 +19335,7 @@
         <v>27</v>
       </c>
       <c r="B71" s="43" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71" s="40" t="s">
@@ -19391,7 +19396,7 @@
         <v>28</v>
       </c>
       <c r="B73" s="43" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="40" t="s">
@@ -19452,7 +19457,7 @@
         <v>29</v>
       </c>
       <c r="B75" s="43" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="40" t="s">
@@ -19508,7 +19513,7 @@
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C77" s="36"/>
       <c r="D77" s="53"/>
@@ -19546,7 +19551,7 @@
         <v>30</v>
       </c>
       <c r="B79" s="43" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="40" t="s">
@@ -19607,7 +19612,7 @@
         <v>31</v>
       </c>
       <c r="B81" s="43" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C81" s="7"/>
       <c r="D81" s="40" t="s">
@@ -19668,7 +19673,7 @@
         <v>32</v>
       </c>
       <c r="B83" s="43" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="40" t="s">
@@ -19729,7 +19734,7 @@
         <v>33</v>
       </c>
       <c r="B85" s="43" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="40" t="s">
@@ -19785,7 +19790,7 @@
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C87" s="36"/>
       <c r="D87" s="53"/>
@@ -19823,7 +19828,7 @@
         <v>34</v>
       </c>
       <c r="B89" s="43" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="40" t="s">
@@ -19884,7 +19889,7 @@
         <v>35</v>
       </c>
       <c r="B91" s="43" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="40" t="s">
@@ -19945,7 +19950,7 @@
         <v>36</v>
       </c>
       <c r="B93" s="43" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93" s="40" t="s">
@@ -20006,7 +20011,7 @@
         <v>37</v>
       </c>
       <c r="B95" s="43" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C95" s="7"/>
       <c r="D95" s="40" t="s">
@@ -20067,7 +20072,7 @@
         <v>38</v>
       </c>
       <c r="B97" s="43" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C97" s="7"/>
       <c r="D97" s="40" t="s">
@@ -20123,7 +20128,7 @@
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C99" s="36"/>
       <c r="D99" s="53"/>
@@ -20161,7 +20166,7 @@
         <v>39</v>
       </c>
       <c r="B101" s="43" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C101" s="7"/>
       <c r="D101" s="40" t="s">
@@ -20222,7 +20227,7 @@
         <v>40</v>
       </c>
       <c r="B103" s="43" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C103" s="7"/>
       <c r="D103" s="40" t="s">
@@ -20283,7 +20288,7 @@
         <v>41</v>
       </c>
       <c r="B105" s="43" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C105" s="7"/>
       <c r="D105" s="40" t="s">
@@ -20344,7 +20349,7 @@
         <v>42</v>
       </c>
       <c r="B107" s="43" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C107" s="7"/>
       <c r="D107" s="40" t="s">
@@ -20400,7 +20405,7 @@
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="34" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C109" s="36"/>
       <c r="D109" s="53"/>
@@ -20438,7 +20443,7 @@
         <v>43</v>
       </c>
       <c r="B111" s="43" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C111" s="21"/>
       <c r="D111" s="40" t="s">
@@ -20521,7 +20526,7 @@
         <v>44</v>
       </c>
       <c r="B113" s="43" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C113" s="21"/>
       <c r="D113" s="40" t="s">
@@ -20604,7 +20609,7 @@
         <v>45</v>
       </c>
       <c r="B115" s="43" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C115" s="21"/>
       <c r="D115" s="40" t="s">
@@ -20671,7 +20676,7 @@
     </row>
     <row r="117" ht="24" customHeight="1">
       <c r="A117" s="62" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B117" s="63"/>
       <c r="C117" s="64"/>
@@ -31342,7 +31347,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{007400C6-00B7-4B43-9B9D-000B00370013}">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{0026006C-00B5-4B53-A5C5-00EE00E700F8}">
             <xm:f>"Enter score"</xm:f>
             <x14:dxf>
               <font/>
@@ -31383,19 +31388,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00110030-0052-481B-8405-00BE00AA00E9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt=" - " showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00020014-00CA-431C-AAD7-0031000E0054}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt=" - " showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$Q$1:$Q$8</xm:f>
           </x14:formula1>
           <xm:sqref>D18 D54 D74 D96</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D1003C-0089-47DF-A41E-000B009C00B7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="Invalid score entered - Score must be one of:&#10;&#10;Very poor&#10;Poor&#10;Moderate&#10;Good&#10;Excellent&#10;N/A" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D60067-0078-4C14-80B7-007F00CB0098}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="Invalid score entered - Score must be one of:&#10;&#10;Very poor&#10;Poor&#10;Moderate&#10;Good&#10;Excellent&#10;N/A" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$Q$1:$Q$8</xm:f>
           </x14:formula1>
           <xm:sqref>D24 D32</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00870037-00BC-4C74-B729-00BB00090060}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="Invalid score entered - Score must be one of:&#10;&#10;Very poor&#10;Poor&#10;Moderate&#10;Good&#10;Excellent&#10;N/A" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007D00E1-0049-4285-BE7A-001400CB0035}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="Invalid score entered - Score must be one of:&#10;&#10;Very poor&#10;Poor&#10;Moderate&#10;Good&#10;Excellent&#10;N/A" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$Q$1:$Q$7</xm:f>
           </x14:formula1>
@@ -31428,7 +31433,7 @@
   <sheetData>
     <row r="1" ht="23.25" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -31436,7 +31441,7 @@
     <row r="2" ht="15.75" customHeight="1">
       <c r="B2" s="59"/>
       <c r="C2" s="34" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" ht="24.75" customHeight="1">
@@ -31474,10 +31479,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="87" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C4" s="88" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" ht="38.25" customHeight="1">
@@ -31486,10 +31491,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="87" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="88" t="s">
         <v>160</v>
-      </c>
-      <c r="C5" s="88" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="6" ht="38.25" customHeight="1">
@@ -31498,10 +31503,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="87" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C6" s="88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" ht="38.25" customHeight="1">
@@ -31510,10 +31515,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="87" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C7" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" ht="38.25" customHeight="1">
@@ -31522,10 +31527,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="88" t="s">
         <v>165</v>
-      </c>
-      <c r="C8" s="88" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
@@ -31568,10 +31573,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="87" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C11" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" ht="51" customHeight="1">
@@ -31580,10 +31585,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="87" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C12" s="88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" ht="38.25" customHeight="1">
@@ -31592,10 +31597,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="87" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C13" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
@@ -31638,10 +31643,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="87" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C16" s="88" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" ht="51" customHeight="1">
@@ -31650,10 +31655,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="87" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C17" s="88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" ht="38.25" customHeight="1">
@@ -31662,10 +31667,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="87" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C18" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" ht="51" customHeight="1">
@@ -31674,10 +31679,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="87" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C19" s="88" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" ht="51" customHeight="1">
@@ -31686,10 +31691,10 @@
         <v>13</v>
       </c>
       <c r="B20" s="87" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C20" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" ht="38.25" customHeight="1">
@@ -31698,10 +31703,10 @@
         <v>14</v>
       </c>
       <c r="B21" s="87" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C21" s="88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" ht="25.5" customHeight="1">
@@ -31710,10 +31715,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="87" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C22" s="88" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" ht="25.5" customHeight="1">
@@ -31722,10 +31727,10 @@
         <v>16</v>
       </c>
       <c r="B23" s="87" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C23" s="88" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" ht="25.5" customHeight="1">
@@ -31734,10 +31739,10 @@
         <v>17</v>
       </c>
       <c r="B24" s="87" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C24" s="88" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
@@ -31780,10 +31785,10 @@
         <v>18</v>
       </c>
       <c r="B27" s="87" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C27" s="88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" ht="38.25" customHeight="1">
@@ -31792,10 +31797,10 @@
         <v>19</v>
       </c>
       <c r="B28" s="87" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C28" s="88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" ht="51" customHeight="1">
@@ -31804,10 +31809,10 @@
         <v>20</v>
       </c>
       <c r="B29" s="87" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C29" s="88" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" ht="38.25" customHeight="1">
@@ -31816,10 +31821,10 @@
         <v>21</v>
       </c>
       <c r="B30" s="87" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C30" s="88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
@@ -31862,10 +31867,10 @@
         <v>22</v>
       </c>
       <c r="B33" s="87" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C33" s="88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" ht="51" customHeight="1">
@@ -31874,10 +31879,10 @@
         <v>23</v>
       </c>
       <c r="B34" s="87" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C34" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" ht="38.25" customHeight="1">
@@ -31886,10 +31891,10 @@
         <v>24</v>
       </c>
       <c r="B35" s="87" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C35" s="88" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
@@ -31932,10 +31937,10 @@
         <v>25</v>
       </c>
       <c r="B38" s="87" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C38" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" ht="63.75" customHeight="1">
@@ -31944,10 +31949,10 @@
         <v>26</v>
       </c>
       <c r="B39" s="87" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C39" s="88" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" ht="38.25" customHeight="1">
@@ -31956,10 +31961,10 @@
         <v>27</v>
       </c>
       <c r="B40" s="87" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C40" s="88" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" ht="63.75" customHeight="1">
@@ -31968,10 +31973,10 @@
         <v>28</v>
       </c>
       <c r="B41" s="87" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C41" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" ht="38.25" customHeight="1">
@@ -31980,10 +31985,10 @@
         <v>29</v>
       </c>
       <c r="B42" s="87" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C42" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
@@ -31992,7 +31997,7 @@
     </row>
     <row r="44" ht="24.75" customHeight="1">
       <c r="A44" s="85" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
@@ -32026,10 +32031,10 @@
         <v>30</v>
       </c>
       <c r="B45" s="87" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C45" s="88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" ht="38.25" customHeight="1">
@@ -32038,10 +32043,10 @@
         <v>31</v>
       </c>
       <c r="B46" s="87" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C46" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" ht="51" customHeight="1">
@@ -32050,10 +32055,10 @@
         <v>32</v>
       </c>
       <c r="B47" s="87" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C47" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" ht="25.5" customHeight="1">
@@ -32062,10 +32067,10 @@
         <v>33</v>
       </c>
       <c r="B48" s="87" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C48" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" ht="12.75" customHeight="1">
@@ -32074,7 +32079,7 @@
     </row>
     <row r="50" ht="24.75" customHeight="1">
       <c r="A50" s="85" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
@@ -32108,10 +32113,10 @@
         <v>34</v>
       </c>
       <c r="B51" s="87" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C51" s="88" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" ht="38.25" customHeight="1">
@@ -32120,10 +32125,10 @@
         <v>35</v>
       </c>
       <c r="B52" s="87" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C52" s="88" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" ht="25.5" customHeight="1">
@@ -32132,10 +32137,10 @@
         <v>36</v>
       </c>
       <c r="B53" s="87" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C53" s="88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" ht="38.25" customHeight="1">
@@ -32144,10 +32149,10 @@
         <v>37</v>
       </c>
       <c r="B54" s="87" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C54" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" ht="25.5" customHeight="1">
@@ -32156,10 +32161,10 @@
         <v>38</v>
       </c>
       <c r="B55" s="87" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C55" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" ht="12.75" customHeight="1">
@@ -32168,7 +32173,7 @@
     </row>
     <row r="57" ht="24.75" customHeight="1">
       <c r="A57" s="85" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
@@ -32202,10 +32207,10 @@
         <v>39</v>
       </c>
       <c r="B58" s="87" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C58" s="88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" ht="38.25" customHeight="1">
@@ -32214,10 +32219,10 @@
         <v>40</v>
       </c>
       <c r="B59" s="87" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C59" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" ht="51" customHeight="1">
@@ -32226,10 +32231,10 @@
         <v>41</v>
       </c>
       <c r="B60" s="87" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C60" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" ht="38.25" customHeight="1">
@@ -32238,10 +32243,10 @@
         <v>42</v>
       </c>
       <c r="B61" s="87" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C61" s="88" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" ht="12.75" customHeight="1">
@@ -32250,7 +32255,7 @@
     </row>
     <row r="63" ht="24.75" customHeight="1">
       <c r="A63" s="85" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
@@ -32284,10 +32289,10 @@
         <v>43</v>
       </c>
       <c r="B64" s="87" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C64" s="88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" ht="25.5" customHeight="1">
@@ -32296,10 +32301,10 @@
         <v>44</v>
       </c>
       <c r="B65" s="87" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C65" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" ht="51" customHeight="1">
@@ -32308,10 +32313,10 @@
         <v>45</v>
       </c>
       <c r="B66" s="87" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C66" s="88" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" ht="12.75" customHeight="1">
@@ -36062,7 +36067,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00E200AB-0038-41F9-BF1D-0072004200F3}">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00D900AA-00AF-4C85-BA0C-004300CF0031}">
             <xm:f>"Enter score"</xm:f>
             <x14:dxf>
               <font/>
@@ -36129,13 +36134,13 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="89" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B1" s="89" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C1" s="89" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -36152,10 +36157,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D3" s="92">
         <f>A4</f>
@@ -36170,14 +36175,14 @@
         <v>6</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D4" s="92">
         <f t="shared" ref="D4:D7" si="12">A4</f>
         <v>29</v>
       </c>
       <c r="E4" s="93" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F4" s="92">
         <f t="shared" ref="F4:F6" si="13">A5</f>
@@ -36192,14 +36197,14 @@
         <v>7</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D5" s="92">
         <f t="shared" si="12"/>
         <v>49</v>
       </c>
       <c r="E5" s="93" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F5" s="92">
         <f t="shared" si="13"/>
@@ -36214,14 +36219,14 @@
         <v>11</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D6" s="92">
         <f t="shared" si="12"/>
         <v>69</v>
       </c>
       <c r="E6" s="93" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F6" s="92">
         <f t="shared" si="13"/>
@@ -36236,7 +36241,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="91" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D7" s="92">
         <f t="shared" si="12"/>

</xml_diff>